<commit_message>
Finalized current sensing circuit values
</commit_message>
<xml_diff>
--- a/Calculations/Power/Buck-Boost_Compensation_Calculations.xlsx
+++ b/Calculations/Power/Buck-Boost_Compensation_Calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghani\Documents\ECE Projects\Variable_Voltage_Controller\Calculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghani\Documents\ECE Projects\Variable_Voltage_Controller\Calculations\Power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEF1611-F65A-4937-B53C-93606D303EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EBD4F5-29F8-45F7-A12E-1B350FDD9763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{58CDA485-075E-4F90-84D5-99C01D61A5C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{58CDA485-075E-4F90-84D5-99C01D61A5C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Find Equation" sheetId="1" r:id="rId1"/>
@@ -1422,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43B830A-39A0-4551-9C36-7610DAEF15E2}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,11 +1451,11 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <f>B2/C2</f>
-        <v>3</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,11 +1467,11 @@
         <v>16.666666666666668</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D16" si="1">B3/C3</f>
-        <v>3.3333333333333335</v>
+        <v>4.166666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1483,11 +1483,11 @@
         <v>18.333333333333336</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>3.666666666666667</v>
+        <v>4.5833333333333339</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1499,11 +1499,11 @@
         <v>20</v>
       </c>
       <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
         <v>5</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,11 +1515,11 @@
         <v>21.666666666666668</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>4.3333333333333339</v>
+        <v>5.416666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1531,11 +1531,11 @@
         <v>23.333333333333336</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>4.666666666666667</v>
+        <v>5.8333333333333339</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1547,11 +1547,11 @@
         <v>25</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1563,11 +1563,11 @@
         <v>26.666666666666668</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>5.3333333333333339</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1579,11 +1579,11 @@
         <v>28.333333333333336</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>5.666666666666667</v>
+        <v>7.0833333333333339</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1595,11 +1595,11 @@
         <v>30</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1611,11 +1611,11 @@
         <v>31.666666666666668</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>6.3333333333333339</v>
+        <v>7.916666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1627,11 +1627,11 @@
         <v>33.333333333333336</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
+        <v>8.3333333333333339</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1643,11 +1643,11 @@
         <v>35</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,11 +1659,11 @@
         <v>36.666666666666671</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>7.3333333333333339</v>
+        <v>9.1666666666666679</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1675,11 +1675,11 @@
         <v>38.333333333333336</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>7.666666666666667</v>
+        <v>9.5833333333333339</v>
       </c>
     </row>
   </sheetData>
@@ -1691,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D0FFC9-6B3D-499B-AA6F-EB044DC5A774}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2040,7 +2040,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <f>B2/C2</f>
+        <f t="shared" ref="D2:D18" si="1">B2/C2</f>
         <v>4.166666666666667</v>
       </c>
     </row>
@@ -2056,7 +2056,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <f>B3/C3</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
@@ -2072,7 +2072,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <f>B4/C4</f>
+        <f t="shared" si="1"/>
         <v>2.7777777777777781</v>
       </c>
     </row>
@@ -2088,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <f>B5/C5</f>
+        <f t="shared" si="1"/>
         <v>2.3809523809523809</v>
       </c>
     </row>
@@ -2104,7 +2104,7 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <f>B6/C6</f>
+        <f t="shared" si="1"/>
         <v>2.0833333333333335</v>
       </c>
     </row>
@@ -2120,7 +2120,7 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <f>B7/C7</f>
+        <f t="shared" si="1"/>
         <v>1.8518518518518521</v>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f>B8/C8</f>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -2152,7 +2152,7 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <f>B9/C9</f>
+        <f t="shared" si="1"/>
         <v>1.5151515151515154</v>
       </c>
     </row>
@@ -2168,7 +2168,7 @@
         <v>12</v>
       </c>
       <c r="D10">
-        <f>B10/C10</f>
+        <f t="shared" si="1"/>
         <v>1.3888888888888891</v>
       </c>
     </row>
@@ -2184,7 +2184,7 @@
         <v>13</v>
       </c>
       <c r="D11">
-        <f>B11/C11</f>
+        <f t="shared" si="1"/>
         <v>1.2820512820512822</v>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <f>B12/C12</f>
+        <f t="shared" si="1"/>
         <v>1.1904761904761905</v>
       </c>
     </row>
@@ -2216,7 +2216,7 @@
         <v>15</v>
       </c>
       <c r="D13">
-        <f>B13/C13</f>
+        <f t="shared" si="1"/>
         <v>1.1111111111111112</v>
       </c>
     </row>
@@ -2232,7 +2232,7 @@
         <v>16</v>
       </c>
       <c r="D14">
-        <f>B14/C14</f>
+        <f t="shared" si="1"/>
         <v>1.0416666666666667</v>
       </c>
     </row>
@@ -2248,7 +2248,7 @@
         <v>17</v>
       </c>
       <c r="D15">
-        <f>B15/C15</f>
+        <f t="shared" si="1"/>
         <v>0.98039215686274517</v>
       </c>
     </row>
@@ -2264,7 +2264,7 @@
         <v>18</v>
       </c>
       <c r="D16">
-        <f>B16/C16</f>
+        <f t="shared" si="1"/>
         <v>0.92592592592592604</v>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
         <v>19</v>
       </c>
       <c r="D17">
-        <f>B17/C17</f>
+        <f t="shared" si="1"/>
         <v>0.87719298245614041</v>
       </c>
     </row>
@@ -2296,7 +2296,7 @@
         <v>20</v>
       </c>
       <c r="D18">
-        <f>B18/C18</f>
+        <f t="shared" si="1"/>
         <v>0.83333333333333337</v>
       </c>
     </row>

</xml_diff>